<commit_message>
arreglo de codigo foreach controlador planeacion
</commit_message>
<xml_diff>
--- a/storage/op/op-carga.xlsx
+++ b/storage/op/op-carga.xlsx
@@ -928,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +984,7 @@
         <v>9</v>
       </c>
       <c r="G2">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -1010,7 +1010,7 @@
         <v>9</v>
       </c>
       <c r="G3">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -1036,7 +1036,7 @@
         <v>9</v>
       </c>
       <c r="G4">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
@@ -1062,7 +1062,7 @@
         <v>9</v>
       </c>
       <c r="G5">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
@@ -1088,7 +1088,7 @@
         <v>9</v>
       </c>
       <c r="G6">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
@@ -1114,7 +1114,7 @@
         <v>9</v>
       </c>
       <c r="G7">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
@@ -1140,7 +1140,7 @@
         <v>9</v>
       </c>
       <c r="G8">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="H8" t="s">
         <v>14</v>
@@ -1166,7 +1166,7 @@
         <v>9</v>
       </c>
       <c r="G9">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="H9" t="s">
         <v>14</v>
@@ -1192,7 +1192,7 @@
         <v>9</v>
       </c>
       <c r="G10">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>
@@ -1218,7 +1218,7 @@
         <v>9</v>
       </c>
       <c r="G11">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="H11" t="s">
         <v>14</v>
@@ -1244,7 +1244,7 @@
         <v>9</v>
       </c>
       <c r="G12">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H12" t="s">
         <v>14</v>
@@ -1270,7 +1270,7 @@
         <v>9</v>
       </c>
       <c r="G13">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="H13" t="s">
         <v>14</v>
@@ -1296,7 +1296,7 @@
         <v>9</v>
       </c>
       <c r="G14">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s">
         <v>14</v>
@@ -1322,7 +1322,7 @@
         <v>9</v>
       </c>
       <c r="G15">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="H15" t="s">
         <v>14</v>
@@ -1348,7 +1348,7 @@
         <v>9</v>
       </c>
       <c r="G16">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="H16" t="s">
         <v>14</v>
@@ -1374,7 +1374,7 @@
         <v>9</v>
       </c>
       <c r="G17">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="H17" t="s">
         <v>14</v>
@@ -1400,7 +1400,7 @@
         <v>9</v>
       </c>
       <c r="G18">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H18" t="s">
         <v>14</v>
@@ -1426,7 +1426,7 @@
         <v>9</v>
       </c>
       <c r="G19">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="H19" t="s">
         <v>14</v>

</xml_diff>